<commit_message>
Presentatie werk en Planning
</commit_message>
<xml_diff>
--- a/Planning/Planning.xlsx
+++ b/Planning/Planning.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="32">
   <si>
     <t>David</t>
   </si>
@@ -92,18 +92,12 @@
     <t>Presentatie Werk</t>
   </si>
   <si>
-    <t>Props for Collectors Building</t>
-  </si>
-  <si>
     <t>City Background and finish of design of the city</t>
   </si>
   <si>
     <t>Interior Collectors Building</t>
   </si>
   <si>
-    <t xml:space="preserve">Enemy_Camera Script </t>
-  </si>
-  <si>
     <t>Implement all scripts together and test tutorial level</t>
   </si>
   <si>
@@ -114,6 +108,18 @@
   </si>
   <si>
     <t xml:space="preserve">Comments </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enemy bug fixing </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Warden </t>
+  </si>
+  <si>
+    <t>The Warden</t>
+  </si>
+  <si>
+    <t>Props for Collectors Building and city</t>
   </si>
 </sst>
 </file>
@@ -216,7 +222,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -238,6 +244,18 @@
     </xf>
     <xf numFmtId="17" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -564,7 +582,7 @@
   <dimension ref="A1:AC42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -578,7 +596,7 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -602,7 +620,7 @@
         <v>6</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:29" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -613,19 +631,19 @@
         <v>21</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="G2" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>21</v>
@@ -676,8 +694,11 @@
       <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
+      <c r="B6" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="C6" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>20</v>
@@ -705,43 +726,58 @@
       <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="9" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:29" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="10" t="s">
         <v>7</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:29" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="11" t="s">
         <v>8</v>
       </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="I12" s="2"/>

</xml_diff>